<commit_message>
Removed redundant functions & globals. Tidying up.
</commit_message>
<xml_diff>
--- a/FaCup/Resources/FinalTeams.xlsx
+++ b/FaCup/Resources/FinalTeams.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darkx\source\repos\FaCup\FaCup\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFBE3DA-8EDF-44EB-A1F8-E645B62FAAC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76633724-CBB7-4547-B3CF-864E0617A8D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15420" yWindow="2145" windowWidth="28650" windowHeight="16005" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15420" yWindow="2145" windowWidth="15690" windowHeight="14085" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TeamsFinal" sheetId="1" r:id="rId1"/>
@@ -3632,7 +3632,7 @@
   <dimension ref="A1:H1035"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>